<commit_message>
commit species identity from gbif
</commit_message>
<xml_diff>
--- a/chatgpt_vekstmedium_2023.11.12/Data/2_processed_data/chatgpt_species_identification.xlsx
+++ b/chatgpt_vekstmedium_2023.11.12/Data/2_processed_data/chatgpt_species_identification.xlsx
@@ -410,7 +410,23 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Aegilops, Puccinia triticina</t>
+          <t>Species mentioned in the text:
+1. Wheat (Triticum aestivum)
+2. Wheat wild relatives from the Aegilops genus:
+   a. Aegilops genus
+   b. Aegilops speltoides
+   c. Aegilops tauschii
+   d. Aegilops sharonensis
+   e. Aegilops vavilovii
+   f. Aegilops umbellulata
+   g. Aegilops peregrina
+   h. Aegilops kotschyi
+   i. Aegilops longissima
+   j. Aegilops cylindrica
+   k. Aegilops ukurunduensis
+   l. Aegilops speltoides var. ligustica
+   m. Aegilops bicornis
+Note: The text does not explicitly mention all the species from the Aegilops genus, only 13 accessions were examined.</t>
         </is>
       </c>
     </row>
@@ -425,7 +441,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Unclear</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -435,13 +451,14 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Puccinia triticina (leaf rust)
-Winter wheat (common wheat)
-Lr9
-Lr19
-Lr22a
-Lr22b
-Lr25</t>
+          <t>- Puccinia triticina (causative agent of leaf rust)
+- common winter wheat breeding lines
+- isogenic lines carrying genes Lr9, Lr19, Lr22a, Lr22b, and Lr25
+- line 99/08-52
+- lines 19/06-108, 82/08-43, and 82/08-35
+- lines with partial race-specific resistance
+- lines with race non-specific resistance
+- lines with "slow rusting" type resistance</t>
         </is>
       </c>
     </row>
@@ -466,7 +483,8 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Zea mays L. (maize)</t>
+          <t>Species mentioned in the text:
+1. Maize (Zea mays L.)</t>
         </is>
       </c>
     </row>
@@ -486,7 +504,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>This study compared the growth and yield of 'Muscat Hamburg' grapes grafted on 'Dog Ridge' rootstock versus self-rooted cuttings. Grafted vines showed better growth, yield, and nutrient content.</t>
+          <t>This study compared the growth and yield of 'Muscat Hamburg' grapes grafted on 'Dog Ridge' rootstock and self-rooted cuttings in Tamil Nadu, India. The grafted vines showed better growth, yield, and nutrient content in the petiole compared to self-rooted cuttings.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -496,9 +514,8 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>- Grape (Vitis vinifera) var. 'Muscat Hamburg'
-- 'Dog Ridge' (Vitis champini) rootstock
-- 'Muscat Hamburg' self-rooted cuttings</t>
+          <t>1. Muscat Hamburg grape variety (Vitis vinifera)
+2. Dog Ridge rootstock (Vitis champini)</t>
         </is>
       </c>
     </row>
@@ -518,7 +535,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>The study investigated the use of silicon preparations on pine and oak seedlings. Spraying with a 2% concentration resulted in increased photosynthetic efficiency and improved growth parameters.</t>
+          <t>Using silicon preparations can promote growth of forest seedlings, particularly oak seedlings affected by oak powdery mildew, and improve their photosynthetic efficiency, biomass, and root nutrition. Spraying with a 2% concentration is most effective.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -528,7 +545,8 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>- Pine (Pinus sylvestris)
+          <t>Species mentioned in the text:
+- Pine (Pinus sylvestris)
 - Oak (Quercus robur)</t>
         </is>
       </c>
@@ -549,7 +567,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>The study investigated the effect of adding phosphogypsum to soil on the growth of pine seedlings. Different mixing variants were tested, showing potential for improving root development. Longer-term observation and testing for heavy metal effects are suggested.</t>
+          <t>The study examined the effects of different soil media mixtures with phosphogypsum formulations on the growth of young pine seedlings in Polish forest conditions. The use of phosphogypsum-based preparations did not have toxic effects on the seedlings, and a mixture of phosphogypsum and organic ash showed positive effects on root development. However, longer-term observations are needed to fully understand the impact. Lower dosages of 1 and 2 t/ha appear to be the most promising. Heavy metal testing and monitoring of the microbiome are recommended.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -559,7 +577,10 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Pinus sylvestris (pine)</t>
+          <t>- Pinus sylvestris (Scots pine)
+- Pinus silvestris (European pine)
+- Organic ash
+- Sewage sludge</t>
         </is>
       </c>
     </row>
@@ -584,9 +605,8 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>- Guppy (Poecilia reticulata)
-- Artemia nauplii
-- Artemia salina</t>
+          <t>1. Guppy (Poecilia reticulata)
+2. Artemia salina (brine shrimp)</t>
         </is>
       </c>
     </row>
@@ -606,7 +626,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>This study examines the growth-survival trade-off in non-phanerophyte species used in coastal dune restoration. Different plant communities exhibit varying trade-offs, influenced by leaf and floral traits. Plant production should focus on species with low survival rates but low sexual reproductive effort. Planning plant production based on this knowledge can improve restoration outcomes while optimizing costs.</t>
+          <t>This study explores the growth-survival trade-off in non-phanerophyte species used in dune restoration. Plant traits like leaf dry matter content and floral displays affect this trade-off. Foredune plant species have higher growth but lower survival rates compared to transition dune species. This trade-off can inform cost-effective ecosystem restoration actions.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -616,10 +636,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>- Phanerophyte species
-- Non-phanerophyte species
-- 13 perennial non-phanerophyte species
-- Foredune and transition dune communities</t>
+          <t>Species mentioned in the following text:
+1. Phanerophyte species
+2. Non-phanerophyte species
+3. Perennial non-phanerophyte species
+4. Plant species of foredune communities
+5. Plant species of transition dune communities</t>
         </is>
       </c>
     </row>
@@ -634,12 +656,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Eelgrass restoration in Sweden led to rapid colonization and recovery of faunal biodiversity and functional diversity, regardless of patch size. Smaller patches can be as effective as larger ones for promoting biodiversity. Monitoring should consider reference and restored areas.</t>
+          <t>Unclear</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -649,8 +666,8 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>1. Eelgrass (Zostera marina)
-2. Invertebrates (not specified)</t>
+          <t>Species mentioned in the text:
+1. Eelgrass (Zostera marina)</t>
         </is>
       </c>
     </row>
@@ -670,7 +687,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>This study explores the relationship between seed production and regeneration of Pinus sibirica using the thin-billed nutcracker as a mediator. The number of nutcracker birds impacts the abundance of seedlings.</t>
+          <t>The study examines the relationship between seed production and the regeneration of Pinus sibirica, finding that the abundance of seedlings is influenced by the number of Nucifraga birds and vice versa.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -681,8 +698,8 @@
       <c r="F11" t="inlineStr">
         <is>
           <t>Species mentioned in the text:
-1. Pinus sibirica (Siberian pine)
-2. Nucifraga caryocatactes macrorhynchos (thin-billed nutcracker)</t>
+1. Pinus sibirica Du Tour (Siberian pine)
+2. Nucifraga caryocatactes macrorhynchos Brehm C L (thin-billed nutcracker)</t>
         </is>
       </c>
     </row>
@@ -697,7 +714,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>This study examines the distribution of carbon in a seagrass called Posidonia oceanica and how it varies during different seasons and depths in the Mediterranean Sea. The results show that deep-water plants store more carbon during summer and have a different cell wall composition in winter.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -707,7 +729,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Posidonia oceanica</t>
+          <t>1. Posidonia oceanica</t>
         </is>
       </c>
     </row>
@@ -732,15 +754,15 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>- Alysson spinosus (digger wasp)
-- Hemipteran nymphs
-- Hemipteran imagines
-- Delphacidae (true hoppers)
-- Cicadellidae (true hoppers)
-- lilac
-- small-leaved linden
-- Metopia argyrocephala (dipteran kleptoparasitic)
-- Sarcophagidae (Diptera)</t>
+          <t>1. Alysson spinosus (digger wasp)
+2. Hemipteran nymphs or imagines
+3. Delphacidae (true hoppers)
+4. Cicadellidae (true hopper)
+5. lilac plant
+6. small-leaved linden plant
+7. Metopia argyrocephala (dipteran kleptoparasitic)
+8. Sarcophagidae (dipteran) 
+9. Alysson melleus (Nearctic digger wasp)</t>
         </is>
       </c>
     </row>
@@ -760,7 +782,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>A study in Central Ethiopia found a high incidence and wide distribution of Cauliflower mosaic virus (CaMV) and Turnip mosaic virus (TuMV) in cabbage, affecting productivity.</t>
+          <t>This study investigates the occurrence of mosaic diseases caused by Cauliflower mosaic virus (CaMV) and Turnip mosaic virus (TuMV) in cabbage fields in Central Ethiopia. The viruses were found to have a high incidence and wide distribution, affecting cabbage productivity.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -770,9 +792,11 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1. Cabbage (Brassica oleracea var. capitata)
-2. Cauliflower mosaic virus (CaMV)
-3. Turnip mosaic virus (TuMV)</t>
+          <t>- Cabbage (Brassica oleracea var. capitata)
+- Cauliflower mosaic virus (CaMV)
+- Turnip mosaic virus (TuMV)
+- "Habesha gomen" cabbage variety
+- "Tikur gomen" cabbage variety</t>
         </is>
       </c>
     </row>
@@ -792,7 +816,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>The study examined the impact of copper-contaminated soils on the growth of barley plants. It found that plant growth was affected by the concentration of copper and the soil's buffering capacity to heavy metals. A regression equation was developed to determine the maximum permissible concentrations of copper in soils.</t>
+          <t>The study examined the impact of copper-contaminated soil on barley plants, finding that plant growth depends on copper concentration and soil buffering capacity, with a variable maximum permissible concentration.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -822,12 +846,19 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Hazelnut husk waste was tested as a growth medium for German primroses. Results showed that it affected aesthetic appearance score and mean flower weight.</t>
+          <t>This study tested using hazelnut shell waste as a growth medium for German primroses. Results showed it had a significant impact on appearance and flower weight.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>1. German primrose (Primula obconica Hance)
+2. Sphagnum moss peat (SMP)
+3. Hazelnut husk waste (HHW)</t>
         </is>
       </c>
     </row>
@@ -847,7 +878,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>The study examined the effects of soil mixtures on the growth and nutritional status of chestnut seedlings. Forest floor and fertilization had positive effects on seedling growth and photosynthetic parameters. Forest floor incorporation in the soil, along with limited addition of certain nutrients, can enhance nutrient adequacy in soil and plants. This method could be a suitable alternative to nutrient management for chestnut seedlings production.</t>
+          <t>Soil mixtures derived from gneiss weathering and forest floor types had positive effects on growth, photosynthesis, and nutrient status of chestnut seedlings. Forest floor application is a viable alternative for nutrient management.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -857,9 +888,11 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>- Castanea sativa Mill. (Chestnut)
-- Forest floor from chestnuts (GN-CFF)
-- Forest floor from evergreen broad-leaved trees (GN-EFF)</t>
+          <t>In the text, the following species are mentioned:
+1. Castanea sativa Mill. (chestnut)
+2. Evergreen broad-leaved trees (mentioned in the context of forest floor types)
+3. Gneiss (type of soil)
+4. Chestnut seedlings</t>
         </is>
       </c>
     </row>
@@ -879,7 +912,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Macroelement distribution and resorption efficiency of Rumex alpinus, an alpine weed, in the Alps and Krkonose mountains were studied, revealing high demand for N, P, and K.</t>
+          <t>This research examines the distribution and resorption efficiency of macroelements in the organs of Rumex alpinus in the Alps and the Giant Mountains. The study found high variability in soil nutrient contents and determined that Rumex alpinus has a high demand for nitrogen, phosphorus, and potassium. However, the plant's resorption efficiency for these macroelements is lower compared to other plants.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -889,7 +922,8 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Rumex alpinus</t>
+          <t>Species mentioned in the text:
+1. Rumex alpinus</t>
         </is>
       </c>
     </row>
@@ -909,7 +943,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>This study shows that the presence of cattle manure and dung beetles improve oak seedling establishment in Mediterranean silvopastoral ecosystems by protecting acorns from predators and improving microhabitat conditions.</t>
+          <t>The study found that applying cattle manure and dung beetles to Mediterranean silvopastoral ecosystems increased oak seedling establishment by improving acorn survival and reducing predation.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -919,14 +953,15 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>1. Cattle
-2. Dung beetles
-3. Invertebrates
-4. Oaks
-5. Grassland layer
-6. Livestock
-7. Wild predators
-8. Rodents</t>
+          <t>- Cattle
+- Dung beetles
+- Invertebrates
+- Oaks
+- Grassland layer
+- Livestock
+- Wild predators
+- Acorns
+- Rodents</t>
         </is>
       </c>
     </row>
@@ -941,12 +976,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>The study examines the application of sustainability practices in Czech Republic guesthouses, with waste sorting and energy-saving measures being the most common.</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -971,7 +1001,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Using the plant defense hormone methyl jasmonate (MeJA) and clonal propagation method somatic embryogenesis (SE) can enhance Norway spruce resistance to a bark-feeding insect, the pine weevil. SE and MeJA independently decreased damage to spruce plants, and together produced even stronger results in terms of reduced damage and increased survival rates. Further research is needed to understand the mechanisms behind these effects.</t>
+          <t>Using a plant defense hormone and a propagation method reduced damage to Norway spruce plants by a bark-feeding insect, showing potential for improved resistance.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -997,7 +1027,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>A study in Hungary identified a strain of 'Candidatus Phytoplasma asteris' in Sempervivum plants, causing unusual symptoms, but the plants recovered after a year.</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1007,10 +1042,10 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>1. Candidatus Phytoplasma asteris
-2. Sempervivum cultivars (Alpha, Purple Passion, Silberkarneol)
-3. Onion yellows phytoplasma
-4. Muscari botryoides aster yellows phytoplasma</t>
+          <t>- Sempervivum species
+- Cultivars Alpha, Purple Passion, and Silberkarneol
+- Onion yellows phytoplasma
+- 'Muscari botryoides' aster yellows phytoplasma</t>
         </is>
       </c>
     </row>
@@ -1030,7 +1065,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Neofusicoccum parvum has been discovered causing canker and dieback on Alnus glutinosa trees in Portugal, the first report of this in Europe.</t>
+          <t>Neofusicoccum parvum, a fungal species, caused canker and dieback on Alnus glutinosa trees in central Portugal, with a 70% incidence rate. Pathogenicity tests confirmed the first report of its impact on A. glutinosa in Portugal and Europe.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1040,7 +1075,8 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Neofusicoccum parvum, Alnus glutinosa</t>
+          <t>- Neofusicoccum parvum 
+- Alnus glutinosa</t>
         </is>
       </c>
     </row>
@@ -1055,12 +1091,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Querciphoma minuta, a fungus, caused branch and stem canker in Platanus x hispanica trees in Germany. It is a potential canker pathogen with a broader host range than previously recognized.</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1070,11 +1101,9 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Species mentioned in the text:
-1. Querciphoma minuta - a fungus within the Camarosporium complex
-2. Platanus x hispanica - London plane trees
-3. Camarosporium complex - a group of fungi within the genus Camarosporium
-4. oak trees - mentioned as the previously known host of Querciphoma minuta</t>
+          <t>1. Querciphoma minuta
+2. Platanus x hispanica (London plane)
+3. Camarosporium complex</t>
         </is>
       </c>
     </row>
@@ -1094,7 +1123,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Study analyzes the quality of Merlot and Blatina grapes and wines in the Trebinje vineyard, concluding that the conditions are suitable for producing high-quality red wines.</t>
+          <t>This paper investigates the quality of Merlot and Blatina grapes and wine in the Trebinje vineyard, demonstrating suitability for producing quality red wines.</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1104,8 +1133,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>1. Merlot grape variety
-2. Blatina grape variety</t>
+          <t>Merlot, Blatina.</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1153,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>This study focuses on soil contamination with heavy metals near a smelter in Kosovo. The high concentrations of heavy metals negatively affect maize plants by reducing activity and chlorophyll content. DNA damage and increased nuclear DNA content were also observed.</t>
+          <t>This text discusses the effects of soil contamination with heavy metals from a smelter in Drenas, Kosovo, on maize plants and the potential ecological implications.</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1135,8 +1163,15 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Species mentioned in the text:
-1. Maize (Zea mays)</t>
+          <t>- Maize plants (Zea mays)
+- Ferronikel smelter
+- Fe (Iron)
+- Cu (Copper)
+- Mn (Manganese)
+- Cr (Chromium)
+- Cd (Cadmium)
+- Ni (Nickel)
+- Pb (Lead)</t>
         </is>
       </c>
     </row>
@@ -1156,7 +1191,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Controlled atmosphere temperature treatment (CATT) at 35 degrees C, 50% CO2, and 10% O2 for 48 hours effectively eliminates cyclamen mites from strawberry transplants, reducing the need for acaricide applications.</t>
+          <t>Controlled atmosphere temperature treatment (CATT) successfully reduced the number of Phytonemus pallidus (cyclamen mite) in strawberry plants by nearly 100%, offering a potential solution for growers to prevent infestations.</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1166,9 +1201,8 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>- Phytonemus pallidus (cyclamen mite)
-- Fragaria x ananassa Duchesne (strawberry)
-- Abamectin (acaricide)</t>
+          <t>1. Phytonemus pallidus (Cyclamen mite)
+2. Fragaria x ananassa Duchesne (Strawberry)</t>
         </is>
       </c>
     </row>
@@ -1188,17 +1222,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Rootstocks in tomato plants can influence the nutritional status that affects yield, potentially improving nutrient capture and pollination in high-yielding varieties. (25 words)</t>
+          <t>This study explores how bumblebees can sense the nutritional status of tomato plants, specifically focusing on the rootstocks and their impact on pollination and yield.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Bumblebees, tomato (Solanum lycopersicum L.)</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -1218,7 +1247,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>The study found that adding green compost to Mars regolith simulant improved potato plant performance, suggesting potential for growing plants in space using extraterrestrial resources.</t>
+          <t>Green compost amendment was found to improve the performance of potato plants grown on Mars regolith simulant as a substrate for cultivation in space.</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1228,13 +1257,12 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>1. Solanum tuberosum (potato)
-2. 'Colomba' (potato variety)
-3. Mars regolith simulant
-4. Green compost
-5. Fluvial sand
-6. Red soil from Sicily
-7. Volcanic soil from Campania</t>
+          <t>1. Potato (Solanum tuberosum L., cv. 'Colomba')
+2. Mars regolith simulant (MMS-1)
+3. Green compost
+4. Fluvial sand
+5. Red soil from Sicily (RS)
+6. Volcanic soil from Campania (VS)</t>
         </is>
       </c>
     </row>
@@ -1254,7 +1282,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>This study investigates the impact of litter leachates from different habitats on the germination of Norway spruce and dwarf pine trees at alpine treeline.</t>
+          <t>Litter leachate affects germination of Norway spruce, but not dwarf pine. Subalpine tall-herb vegetation serves as a filter, impacting woody species seedling composition.</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1266,7 +1294,7 @@
         <is>
           <t>- Norway spruce (Picea abies)
 - Dwarf pine (Pinus mugo)
-- Calamagrostis villosa (a dominant plant in subalpine tall-herb vegetation)</t>
+- Calamagrostis villosa</t>
         </is>
       </c>
     </row>
@@ -1286,12 +1314,20 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Passerine birds play a vital role in the seed dispersal of Vaccinium species in managed forests, with the birds depositing viable seeds on tree stumps, which create favorable conditions for seedling establishment. However, environmental factors greatly impact this process.</t>
+          <t>Passerine birds in the boreal forest help facilitate seed dispersal and sexual reproduction for Vaccinium shrubs by depositing seeds in tree stumps, providing suitable conditions for seedling establishment.</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Species mentioned in the text:
+1. Vaccinium shrubs (keystone species)
+2. Passerine birds (seed dispersers)
+3. Bryophytes (required for seedling establishment)</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1347,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Industrial hemp plants have natural resistance to insect pests due to their physical strength and chemical composition. Insects that do attack hemp are general pests found in many farming systems. Effective management options exist.</t>
+          <t>Industrial hemp plants have natural resistance to many insect pests due to their physical strength and chemical composition. However, there are still some pests that can cause damage, including cotton bollworm and native budworm. Other sporadic pests include leaf beetles, mirids, and seed-collecting ants. Effective management options include organic, biological, and conventional methods.</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1321,18 +1357,18 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>1. Cotton bollworm (Helicoverpa armigera)
-2. Native budworm (H. punctigera)
-3. Rutherglen bug (Nysius vinitor)
-4. Green vegetable bug (Nezara viridula)
-5. Leaf beetles (Monoleptis australis)
-6. Mirids (Creontiades pallida)
-7. Stem borer (cerambycid beetle)
-8. Seed-collecting ants
-9. Wireworms
-10. Red-legged earth mite (Halotydeus destructor)
-11. Cabbage white butterflies (Pieris rapae)
-12. Miscellaneous grass moths</t>
+          <t>- cotton bollworm (Helicoverpa armigera)
+- native budworm (H. punctigera)
+- Rutherglen bug (Nysius vinitor)
+- green vegetable bug (Nezara viridula)
+- leaf beetles (Monoleptis australis)
+- mirids (Creontiades pallida)
+- stem borer (cerambycid beetle)
+- seed-collecting ants
+- wireworms
+- red-legged earth mite (Halotydeus destructor)
+- cabbage white butterflies (Pieris rapae)
+- miscellaneous grass moths</t>
         </is>
       </c>
     </row>
@@ -1352,7 +1388,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Thirteen populations of wild garlic were found in Western Serbia, growing in eight different soil types. The populations on Povlen and Rudnik mountains had the most productive morphological parameters.</t>
+          <t>The study measured morphological parameters of Allium ursinum populations in Western Serbia and found that the populations on mountains Povlen and Rudnik have the most productive parameters for agricultural research.</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1362,7 +1398,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Allium ursinum L.</t>
+          <t>Allium ursinum</t>
         </is>
       </c>
     </row>
@@ -1382,7 +1418,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>The study examined the impact of nitrogen levels and cultivars on yield and yield components of radicchio. Results showed that the highest fresh weight was achieved with 150 kg N/ha. Increasing soil nitrogen supply led to decreased dry matter content and firmness of radicchio heads.</t>
+          <t>Field experiments in Slovenia found that nitrogen application levels and cultivars did not interact in their effect on radicchio yield and yield components. The highest fresh weight was achieved with 150 kg N/ha, but dry matter content and firmness of radicchio heads decreased with increased soil N supply. N levels did not significantly affect leaf number.</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1392,13 +1428,20 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>1. Radicchio
-2. 'Monivip' (cultivar)
-3. 'Castel Franco' (cultivar)
-4. 'Anivip' (cultivar)
-5. 'Foresto' (cultivar)
-6. 'Palla rossa' (cultivar)
-7. 'Verona' (cultivar)</t>
+          <t>The different species mentioned in the text are:
+1. Nitrogen
+2. Radicchio
+3. Biotechnical centre
+4. Naklo
+5. Kranj
+6. Slovenia
+7. Cultivars: 'Monivip', 'Castel Franco', 'Anivip', 'Foresto', 'Palla rossa', and 'Verona'
+8. Headed chicory
+9. KAN (calcium ammonium nitrate)
+10. Calcium
+11. Amonium
+12. Fertilizers
+13. Crop</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1456,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Unclear</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1423,14 +1466,14 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>1. Sycamore (Acer pseudoplatanus)
-2. Boxelder maple (Acer negundo)
-3. Silver maple (Acer saccharinum)
-4. Sugar maple (Acer saccharum)
-5. Japanese maple (Acer palmatum)
-6. Trident maple (Acer buergerianum)
-7. Paperbark maple (Acer griseum)
-8. Himalayan maple (Acer oblongum)</t>
+          <t>- Sycamore (Acer pseudoplatanus)
+- Boxelder maple (Acer negundo)
+- Silver maple (Acer saccharinum)
+- Sugar maple (Acer saccharum)
+- Japanese maple (Acer palmatum)
+- Trident maple (Acer buergerianum)
+- Paperbark maple (Acer griseum)
+- Himalayan maple (Acer oblongum)</t>
         </is>
       </c>
     </row>
@@ -1450,7 +1493,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>A study was conducted to evaluate the leafiness of Festuca species, varieties, and ecotypes and select the most suitable for breeding based on their forage quality. Accessions from local and foreign origins were collected and analyzed. The study found significant variation in leafiness, with the accessions categorized as low, medium, or strong leafy. On average, the variety Albena had the highest leafiness at 59.54%.</t>
+          <t>Breeding assessment of leafiness in Festuca species for forage quality. Evaluation of species, varieties, and ecotypes to select high leafy accessions. Variations in leafiness and the leafiest variety is tall fescue Albena at 59.54%.</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1461,9 +1504,9 @@
       <c r="F36" t="inlineStr">
         <is>
           <t>Species mentioned in the text:
-1. Tall fescue
-2. Meadow fescue
-3. Red fescue</t>
+- Tall fescue
+- Meadow fescue
+- Red fescue</t>
         </is>
       </c>
     </row>
@@ -1483,7 +1526,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>The study focused on determining the phenolic composition of plum fruits grown in Tambov oblast. Various phenolic compounds, including hydroxycinnamic acids, anthocyanins, and flavonols, were identified in the fruits.</t>
+          <t>Study focused on determining the phenolic composition of plum fruits grown in Tambov oblast, Russia using high performance liquid chromatography. Plum fruits were found to be a potential source of phenolic compounds.</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1493,17 +1536,16 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>1. Prunus domestica L. (plum)
-2. Prunus domestica hexaploid species (plum)
-3. Plum-cherry hybrid (SVG) 11-19 (plum-cherry hybrid)
-4. 4-Caffeoylquinic acid (phenolic compound)
-5. 5-Caffeoylquinic acid (phenolic compound)
-6. 3-p-Coumaroylquinic acid (phenolic compound)
-7. 3-Caffeoylquinic acid (phenolic compound)
-8. Quercitin-3-rutinoside (flavonol)
-9. Cyanidin-3-glucoside (anthocyanin)
-10. Cyanidin-3-rutinoside (anthocyanin)
-11. Peonidin-3-glucoside (anthocyanin)</t>
+          <t>- Prunus domestica L. (Plum)
+- SVG 11-19 (Plum-cherry hybrid)
+- 4-Caffeoylquinic acid
+- 5-Caffeoylquinic acid
+- 3-p-Coumaroylquinic acid
+- 3-Caffeoylquinic acid
+- Quercitin-3-rutinoside
+- Cyanidin-3-glucoside
+- Cyanidin-3-rutinoside
+- Peonidin-3-glucoside</t>
         </is>
       </c>
     </row>
@@ -1528,7 +1570,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Species mentioned in the text: Salvia yangii, Salvia abrotanoides</t>
+          <t>Salvia yangii, Salvia abrotanoides</t>
         </is>
       </c>
     </row>
@@ -1553,15 +1595,10 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Species mentioned in the text:
-1. Lemon (Citrus limon)
-2. Mikrokarpo Messaras (lemon cultivar)
-3. Nouvel Athos (lemon cultivar)
-4. Femminello Commune (lemon cultivar)
-5. Zia gara Bianca (lemon cultivar)
-6. Sour Orange (Citrus aurantium)
-7. Yuma Ponderosa lemon (Citrus limon)
-8. Volkameriana (rootstock, specific species not mentioned, but likely Citrus volkameriana)</t>
+          <t>1. Lemon (Citrus limon)
+2. Sour Orange (Citrus aurantium)
+3. Yuma Ponderosa lemon (Citrus x jambhiri)
+4. Volkameriana (Citrus volkameriana)</t>
         </is>
       </c>
     </row>
@@ -1586,8 +1623,8 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>- Apple
-- Bramley's Seedling
+          <t>- Apple 
+- Bramley's Seedling 
 - Falstaff</t>
         </is>
       </c>
@@ -1608,7 +1645,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>This study aimed to evaluate seed weight and imbibition period for three peony species native to Serbia, providing preliminary research for future germination studies.</t>
+          <t>This study examined seed weight and imbibition period of herbaceous peony species native to Serbia, providing preliminary research for future peony germination studies.</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1618,9 +1655,9 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Paeonia tenuifolia (fern leaf peony or steppe peony)
-Paeonia peregrina (Balkan peony or Kosovo peony)
-Paeonia daurica Andrews</t>
+          <t>- Paeonia tenuifolia (fern leaf peony or steppe peony)
+- Paeonia peregrina (Balkan peony or Kosovo peony)
+- Paeonia daurica</t>
         </is>
       </c>
     </row>
@@ -1640,7 +1677,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>This study examines the effects of cultivar and plant origin on minituber production in aeroponics. Agria plants of minituber origin produced the highest yield of minitubers.</t>
+          <t>This study evaluated the effects of cultivar and plant origin on minituber production in an aeroponic facility. Agria plants of minituber origin had the highest yield and heaviest tubers.</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1650,9 +1687,9 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>1. Potato (Solanum tuberosum)
-2. Sinora (potato cultivar)
-3. Agria (potato cultivar)</t>
+          <t>- Potato (Solanum tuberosum)
+- Sinora (Potato cultivar)
+- Agria (Potato cultivar)</t>
         </is>
       </c>
     </row>
@@ -1672,7 +1709,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Salinity affects the growth and functioning of meadow buttercup. It cannot establish in habitats with high salinity, but grows best in subsaline habitats. Salinity hampers growth and photosynthesis.</t>
+          <t>The study found that sodic salinity negatively affects the growth and functioning of the meadow buttercup. The species is best adapted to subsaline habitats and shows limitations at higher salinities. Increases in salinity hampered growth, leaf morphology, and photosynthesis, but not mineral nutrition. Leaf appearance can be a sign of progressing salinity. Ultimately, rising salinity reduces the competitiveness of the species and shifts its strategy to ruderal behavior.</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1682,7 +1719,8 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>- Meadow buttercup (Ranunculus acris L.)</t>
+          <t>Species mentioned in the text:
+1. Meadow buttercup (Ranunculus acris L.)</t>
         </is>
       </c>
     </row>
@@ -1707,8 +1745,8 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>- Coastal Douglas-fir (Pseudotsuga menziesii)
-- Interior Douglas-fir (Pseudotsuga menziesii)</t>
+          <t>1. Coastal Douglas-fir (Pseudotsuga menziesii)
+2. Interior Douglas-fir (Pseudotsuga menziesii)</t>
         </is>
       </c>
     </row>
@@ -1728,7 +1766,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Infested sawdust can pose a risk to pine seedlings as pinewood nematodes actively move from the sawdust into damaged roots and stems, causing infestation.</t>
+          <t>The study aimed to assess if pine seedlings could be infested with pinewood nematodes through sawdust. Findings showed that nematodes can move from infested sawdust into damaged seedlings.</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1738,9 +1776,9 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>1. Pine (Pinus sylvestris L.)
-2. Pinewood nematode (Bursaphelenchus xylophilus Steiner and Buhrer (Nickle))
-3. Beetles of the genus Monochamus</t>
+          <t>- Pine (Pinus sylvestris L.)
+- Pinewood nematode (Bursaphelenchus xylophilus Steiner and Buhrer)
+- Beetles of the genus Monochamus</t>
         </is>
       </c>
     </row>
@@ -1760,17 +1798,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>This study explores the potential of seed treatments for improving lucerne seed performance and early growth. Various treatments were tested, with potassium permanganate and chitosan showing the best results for seedling length and emergence. Bentonite and gypsum were recommended for root development. Cinnamon powder improved emergence, seedling, and shoot length. The combination of priming and coating methods appeared to be the most effective, especially in field conditions.</t>
+          <t>Various seed treatments, including heat treatment, seed priming, and seed coating, were tested for their potential to improve lucerne seed performance and early field growth. Seed priming with potassium permanganate and chitosan showed the best results for seedling length and emergence dynamics, while coating with bentonite and gypsum had a positive impact on root development. Cinnamon powder improved emergence dynamics, seedling, and shoot length. The combination of priming and coating methods was found to be the most effective in field conditions.</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>- Lucerne (also known as alfalfa)</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -1790,7 +1823,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>The study analyzed the impact of different seedling ages and cultivation methods on the quality and yield of sweet pepper plants. Results showed that 60-day-old seedlings had better growth and leaf characteristics, while 40-day-old seedlings had higher photosynthetic parameters. Higher yields were observed in 60-day-old seedlings directly sown in cups.</t>
+          <t>The age of sweet pepper seedlings and the cultivation method have an impact on seedling quality and productivity. 60-day-old seedlings grown by transplanting had higher yield.</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1800,7 +1833,8 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Capsicum annuum L. (sweet pepper)</t>
+          <t>Species mentioned in the text:
+1. Sweet pepper (Capsicum annuum L.)</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1849,12 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Cd and Pb content in herbs and spices used in Polish cuisine was examined. The results showed low risk of toxicity, but some products exceeded acceptable limits and should be consumed with caution.</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1825,17 +1864,17 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>The different species mentioned in the text are:
-- Dried herbs: 9 kinds (specific herbs not mentioned)
-- Fresh herbs: 15 kinds (specific herbs not mentioned)
-- Single-component spices: 14 kinds (specific spices not mentioned)
-- Coriander
-- Estragon
-- Watercress
-- Jiaogulan
-- Celery
-- Basil
-- Dill</t>
+          <t>species mentioned:
+- dried herbs
+- fresh herbs
+- loose single-component spices
+- coriander
+- estragon
+- watercress
+- jiaogulan
+- celery
+- basil
+- dill</t>
         </is>
       </c>
     </row>
@@ -1850,12 +1889,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Different assays were used to evaluate the resistance of grapevine cultivars to Eutypa dieback. Assays 1 and 2 were more consistent in assessing resistance compared to Assay 3.</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1865,8 +1899,18 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>1. Eutypa lata (causal fungus)
-2. Vitis vinifera cultivars: 'Black Corinth', 'Carignane', 'Husseine', 'Merlot', 'Muscat Hamburg', 'Palomino', 'Peloursin', 'Primitivo' (aka 'Zinfandel'), and 'Thompson Seedless'</t>
+          <t>- Vitis vinifera cultivars:
+  - Black Corinth
+  - Carignane
+  - Husseine
+  - Merlot
+  - Muscat Hamburg
+  - Palomino
+  - Peloursin
+  - Primitivo (aka Zinfandel)
+  - Thompson Seedless
+- Causal fungus:
+  - Eutypa lata</t>
         </is>
       </c>
     </row>
@@ -1891,9 +1935,8 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>- European pear (Pyrus communis L.)
-- Quince clonal rootstocks (Province Quince BA29 [BA29], Quince A [QA], and Quince MC [MC])
-- Pear cultivars: 'Deveci', 'Williams', 'Santa Maria' and 'Abate Fetel'</t>
+          <t>- Quince clonal rootstocks (Province Quince BA29 [BA29], Quince A [QA], and Quince MC [MC])
+- European pear (Pyrus communis L.) cultivars: 'Deveci', 'Williams', 'Santa Maria', and 'Abate Fetel'</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1956,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>The study analyzed the drought resistance of different garden rose genotypes. The genotypes 'Borisfen' and R. hugonis showed the best water-holding and recovery capabilities under water stress conditions. They also had stable functioning of chlorophyll fluorescence induction parameters. Other genotypes showed instability and irreversible metabolic disturbances. Overall, 'Borisfen' and R. hugonis had the highest drought tolerance.</t>
+          <t>Physiological and biochemical characteristics of drought tolerance in different garden rose genotypes were studied. The best water-holding capabilities were found in cv. 'Borisfen' and R. hugonis species, while R. indica, R. bracteata, R. rouletti, R. foetida showed instability. Recovery of metabolic processes was observed in R. hugonis, R. bracteata, R. indica, and cv. 'Borisfen' after mild wilting, but irreversible disturbances occurred in R. gallica, R. indica, and R. bracteata under severe wilting conditions. The highest drought tolerance was found in cv. 'Borisfen' and R. hugonis.</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1923,13 +1966,13 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>1. cv. 'Borisfen'
-2. R. hugonis
-3. R. indica
-4. R. bracteata
-5. R. rouletti
-6. R. foetida
-7. R. gallica</t>
+          <t>- Garden roses (genotypes)
+- R. hugonis
+- R. indica
+- R. bracteata
+- R. rouletti
+- R. foetida
+- R. gallica</t>
         </is>
       </c>
     </row>
@@ -1949,12 +1992,20 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>A study compared biodegradable mulching film and traditional polyethylene film on tomato yield and quality. Both films increased yield and improved fruit quality, making them a sustainable alternative.</t>
+          <t>Biodegradable mulching film increases tomato yield and quality. Both types of film tested (biodegradable and polyethylene) showed positive effects, with biodegradable film being more sustainable.</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>1. San Marzano tomato
+2. Flavonoids
+3. Polyphenols
+4. AsA (Ascorbic acid)</t>
         </is>
       </c>
     </row>
@@ -1974,7 +2025,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>This study examines the accumulation and translocation of copper in grapevine grafts depending on rootstocks and growing media. Both rootstocks showed exclusive accumulation of copper. Soils with high copper content hindered graft growth.</t>
+          <t>This study investigated the accumulation and translocation of copper in grapevine grafts grown in different soil media. Both rootstocks showed high copper accumulation, with SO4 rootstock having a higher translocation rate. Soil with high copper content was found to inhibit graft growth.</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1984,10 +2035,10 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>- Grapevine (Vitis vinifera)
-- Sauvignon Blanc (grape variety)
-- 5BB (rootstock)
-- SO4 (rootstock)</t>
+          <t>- Grapevine
+- Sauvignon Blanc
+- 5BB rootstock
+- SO4 rootstock</t>
         </is>
       </c>
     </row>
@@ -2007,7 +2058,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Sea buckthorn, a shrub found in Romania, has various uses in agriculture, medicine, and forestry due to its high nutritional value and environmental benefits. It is important to protect this natural resource to prevent its disappearance.</t>
+          <t>Sea buckthorn is a valuable shrub in Romania, with numerous uses including food, medicine, and forestry. It has high nutritional value and can improve the climate and prevent pollution.</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2017,7 +2068,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>1. Sea buckthorn (Hippophae rhamnoides)</t>
+          <t>Hippophae rhamnoides (Sea buckthorn)</t>
         </is>
       </c>
     </row>
@@ -2037,7 +2088,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Bark and wood traits of different tree species influence invertebrate communities in mid-decay logs. Maintaining deadwood heterogeneity is important for biodiversity. Bark exchange method can track bark trait effects.</t>
+          <t>Reciprocal bark exchange between tree species reveals that both bark and wood have different effects on invertebrate communities in mid-decay logs, emphasizing the importance of maintaining deadwood heterogeneity.</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2047,11 +2098,11 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>- Araucaria araucana
-- Cryptomeria japonica
-- Picea abies
-- Thuja plicata
-- Chamaecyparis lawsoniana</t>
+          <t>1. Araucaria araucana
+2. Cryptomeria japonica
+3. Picea abies
+4. Thuja plicata
+5. Chamaecyparis lawsoniana</t>
         </is>
       </c>
     </row>
@@ -2071,7 +2122,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>This study compared the chemical composition, antioxidant activity, and polyphenolic compounds in garlic leaves and bulbs, finding that leaves contained higher levels of certain compounds and antioxidants.</t>
+          <t>The study compared the chemical composition and antioxidant activity of garlic leaves and bulbs at different stages of development. Garlic leaves contained more protein, fat, ash, vitamin C, and polyphenols than bulbs. Young plants had higher levels of bioactive compounds.</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2081,12 +2132,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>- Garlic (Allium sativum)
-- Winter garlic plants (Allium sativum)
-- Harnas cultivar (Allium sativum)
-- Ornak cultivar (Allium sativum)
-- Catechin
-- Epicatechin</t>
+          <t>1. Garlic (Allium sativum)</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2147,12 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Tomato yellow leaf curl Sardinia virus (TYLCSV) does not transmit through tomato seeds, as genetic material was not detected in seedlings or embryos.</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2111,11 +2162,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Species mentioned in the text:
-1. Tomato (Solanum lycopersicum)
-2. Tomato yellow leaf curl Sardinia virus (TYLCSV)
-3. Geminiviruses (family: Geminiviridae)
-4. Hemipteran insects (order: Hemiptera)</t>
+          <t>Tomato yellow leaf curl Sardinia virus, tomato</t>
         </is>
       </c>
     </row>
@@ -2135,7 +2182,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>This study investigates the use of seed-propagated plug plants in Miscanthus cultivation, exploring the effects of plug size, sowing date, and seedling age on field establishment and yield.</t>
+          <t>Using seed-propagate plug plants of Miscanthus can improve propagation rates and scale up of plantations, while plug design and planting date have significant effects on yield and establishment rates.</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2170,7 +2217,8 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Posidonia oceanica</t>
+          <t>Species mentioned in the text:
+1. Posidonia oceanica (seagrass)</t>
         </is>
       </c>
     </row>
@@ -2190,7 +2238,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Albizia richardiana contains phytotoxic compounds that can be used as bioherbicides to control weeds. Three active compounds were isolated and shown to suppress plant growth.</t>
+          <t>Research on Albizia richardiana plant revealed three phytotoxic compounds that can be used as bioherbicides to control weeds, potentially reducing the need for synthetic chemical herbicides.</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2200,11 +2248,10 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Species mentioned in the text:
-1. Albizia richardiana (plant)
-2. Lettuce (Lactuca sativa)
-3. Italian ryegrass
-4. Lepidium sativum (cress)</t>
+          <t>1. Albizia richardiana (plant species)
+2. Lettuce (weed species)
+3. Italian ryegrass (weed species)
+4. Lepidium sativum (cress) (weed species)</t>
         </is>
       </c>
     </row>
@@ -2224,7 +2271,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Growing crop mixtures can increase insect biodiversity and abundance, benefiting ecosystem services such as pollination and pest control without compromising crop yield.</t>
+          <t>Crop mixtures, specifically those containing faba bean, linseed, or oilseed rape, can increase arthropod biodiversity and abundance, supporting pollination and pest-control ecosystem services without compromising crop yield.</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2234,10 +2281,16 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>- Wheat
+          <t>The different species mentioned in the text are:
+- Arthropods
+- Wheat
 - Faba bean
 - Linseed
-- Oilseed rape</t>
+- Oilseed rape
+- Grassland biodiversity organisms
+- Mass-flowering crops
+- Legumes
+- Cereals</t>
         </is>
       </c>
     </row>
@@ -2257,7 +2310,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Researchers studied the recovery and formation of soil microbiomes in forest plantations after disturbances in a dry-steppe zone, finding different rates of restoration and formation among burnt and provenance trial sites.</t>
+          <t>The study examines the recovery and formation of biological soil properties in forest plantations after disturbances such as wildfires using microbiological indicators.</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2267,7 +2320,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Pinus sylvestris (Scots pine), Larix sibirica (Siberian larch), Ulmus humilis (field elm), P. sibirica (Siberian pine), P. sylvestris (Scots pine).</t>
+          <t>Pinus sylvestris, Larix sibirica, Ulmus humilis</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2365,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>This study examines the formation of potato yield based on agricultural techniques in Forest-Steppe conditions, focusing on soil type, fertilization, and seed tuber characteristics. Optimal practices for high-quality planting material and profitable agribusiness are identified.</t>
+          <t>Optimizing plant nutrition and cultivation methods can maximize potato yield. The study examines the growth and development of different potato varieties in Forest-Steppe conditions, finding that yield depends on fertilization, planting tuber fraction, and variety characteristics. Maximum yield is achieved with specific fertilization methods and using seed tubers of a certain size. The findings can be applied to improve seed potato production and agribusiness profitability.</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2322,9 +2375,9 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>- Laperla (potato variety)
-- Granada (potato variety)
-- Memphis (potato variety)</t>
+          <t>- Laperla
+- Granada
+- Memphis</t>
         </is>
       </c>
     </row>
@@ -2344,7 +2397,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Fungi from Thailand have been found to successfully biodegrade low-density polyethylene (LDPE) film, suggesting their potential use in plastic degradation systems.</t>
+          <t>Fungi from Thailand were tested for their ability to biodegrade low-density polyethylene (LDPE) films. Several fungi showed significant growth and degradation of LDPE films, indicating their potential use in plastic degradation.</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2354,11 +2407,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>1. Diaporthe italiana
-2. Thyrostroma jaczewskii
-3. Collectotrichum fructicola
-4. Stagonosporopsis citrulli
-5. Aspergillus niger</t>
+          <t>Diaporthe italiana, Thyrostroma jaczewskii, Collectotrichum fructicola, Stagonosporopsis citrulli, Aspergillus niger</t>
         </is>
       </c>
     </row>
@@ -2383,9 +2432,9 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>- Lemon (Citrus x limon)
-- Neofusicoccum parvum
-- Citrange (C. sinensis x Poncirus trifoliata) 'Carrizo' rootstock</t>
+          <t>Citrus x limon (lemon)
+Neofusicoccum parvum
+Citrus sinensis x Poncirus trifoliata (citrange)</t>
         </is>
       </c>
     </row>
@@ -2405,7 +2454,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Isaria fumosorosea is not effective against the box tree moth, possibly due to host plant chemicals inhibiting fungus growth on the pest's cuticle.</t>
+          <t>The efficacy of Isaria fumosorosea against the box tree moth is low. Host plant phytochemicals may be involved in the moth's defense against fungal pathogens.</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2416,9 +2465,9 @@
       <c r="F67" t="inlineStr">
         <is>
           <t>- Isaria fumosorosea
-- Cydalima perspectalis (box tree moth)
-- Buxus sp. (box tree)
-- B. sempervirens (common box)</t>
+- Cydalima perspectalis
+- Buxus sp.
+- B. sempervirens</t>
         </is>
       </c>
     </row>
@@ -2433,7 +2482,12 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Defaunation caused by hunting in French Guiana's rainforests is affecting the functional composition of tree communities, resulting in shifts in leaf and fruit traits and wood density. These changes have long-term ecological consequences.</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2443,10 +2497,12 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Species mentioned in the text include:
-- Tropical vertebrate populations
+          <t>- Tropical vertebrate populations
+- Seed dispersers
+- Predators
+- Browsers
 - Tree recruits
-- Adults</t>
+- Tree adults</t>
         </is>
       </c>
     </row>
@@ -2466,7 +2522,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>This study explores the relationship between competition, productivity, and biomass in plant communities, focusing on different types of growing media. Competition for survival increases with community biomass, while competition for growth increases with productivity in high-biomass communities. The confusion between productivity and biomass has contributed to the debate on competition and diversity.</t>
+          <t>Research explores the relationship between competition and productivity in plant communities, highlighting the confusion between productivity and biomass and the need for further study in this area. The study also examines traits that explain competition and its correlation with diversity.</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2486,7 +2542,12 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>The study investigates the impact of fish waste on feeding and reproductive ability in Iceland scallops. Results show some differences in feeding but no significant effects on reproductive ability.</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2496,7 +2557,12 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>1. Iceland scallop (Chlamys islandica)</t>
+          <t>Species mentioned in the text:
+1. Iceland scallop (Chlamys islandica)
+2. Norwegian salmon (Salmo salar)
+3. Arctic species
+4. Subarctic species
+5. Finfish (unspecified species)</t>
         </is>
       </c>
     </row>
@@ -2516,7 +2582,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>This study compares the chemical composition of soil and the Syringa vulgaris plant in abandoned cemeteries. It found no significant differences between burial and non-burial areas.</t>
+          <t>This study compared the chemical composition of Syringa vulgaris (lilac) and soil in abandoned cemeteries. The plant's tissue composition was more influenced by soil substrate and formation process than burial sites.</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2526,18 +2592,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>- Syringa vulgaris (Lilac)
-- Ca (Calcium)
-- Na (Sodium)
-- Mg (Magnesium)
-- Al (Aluminum)
-- Fe (Iron)
-- Zn (Zinc)
-- Cd (Cadmium)
-- Pb (Lead)
-- K (Potassium)
-- C (Carbon)
-- P (Phosphorus)</t>
+          <t>Syringa vulgaris (lilac), Ca, Na, Mg, Al, Fe, Zn, Cd, Pb</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2612,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Real-time PCR was used to detect and quantify oomycetes (Phytophthora, Pythium, and Phytopythium) in ornamental nursery stock. Oomycetes were found in all plants tested, with higher amounts in compost.</t>
+          <t>Real-time PCR was used to detect and quantify oomycetes in ornamental plants bought from various sources. Oomycete DNA was found in composts, roots, and filters, with the highest quantities detected using the ITS probe. No differences were found between plants purchased online or from traditional retailers.</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2587,7 +2642,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Warmer temperatures during reproduction induce significant transcriptomic differences in strawberry ecotypes, with more variation in asexual reproduction and few genes shared between ecotypes. The epigenetic machinery is affected differently during asexual and sexual reproduction.</t>
+          <t>Study investigates the effects of warmer temperatures on the transcriptomes of different strawberry ecotypes during asexual and sexual reproduction, highlighting differences in gene expression and splicing isoforms.</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2597,7 +2652,10 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Fragaria vesca (strawberry)</t>
+          <t>1. Fragaria vesca (strawberry)
+2. SOC1
+3. LHY
+4. SVP</t>
         </is>
       </c>
     </row>
@@ -2617,7 +2675,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>The study focused on the volatile profiles of arborvitae trees suffering from drought and insect infestation, specifically the cypress bark beetle. Differences in volatiles were found between healthy, dehydrated, and infested trees. Further research is needed to understand the behavioral role of these volatiles.</t>
+          <t>Changes in volatile profiles of arborvitae from drought and insect infestation were analyzed. Key components specific to stressed trees were identified, which could be useful for pest management.</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2629,20 +2687,21 @@
         <is>
           <t>1. Arborvitae (Thuja occidentalis)
 2. Cypress bark beetle (Phloeosinus aubei)
-3. Cupressaceae 
-4. Coleoptera 
-5. Curculionidae 
-6. Scolytinae 
-7. Pinene 
-8. Thujene 
-9. Thujone 
-10. Beta-pinene 
-11. Myrcene 
-12. Limonene 
-13. P-cymene 
-14. Camphene 
-15. Fenchene 
-16. Fenchone</t>
+3. Coleoptera
+4. Curculionidae
+5. Scolytinae
+6. Cupressaceae
+7. Pinene (a-pinene)
+8. Thujene (a-thujene)
+9. Thujone (a-thujone)
+10. Beta-pinene
+11. Myrcene
+12. Limonene
+13. P-cymene
+14. Camphene
+15. Fenchene
+16. Frass
+17. Fenchone</t>
         </is>
       </c>
     </row>
@@ -2667,13 +2726,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Species mentioned in the text:
-1. Salvia fruticosa
-2. Malva sylvestris
-3. Taraxacum officinale
-4. Plantago ovata
-5. Tanacetum parthenium
-6. Allium sativum</t>
+          <t>Salvia fruticosa, Malva sylvestris, Taraxacum officinale, Plantago ovata, Tanacetum parthenium, Allium sativum</t>
         </is>
       </c>
     </row>
@@ -2688,7 +2741,12 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>First report of canna yellow streak virus in Iran's canna plants causing severe symptoms. The virus is similar to isolates from Russia and UK.</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2698,10 +2756,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>- Canna indica (canna)
-- Potyvirus
-- canna yellow streak virus (CaYSV)
-- Cannaceae family</t>
+          <t>Canna indica, Potyvirus, canna yellow streak virus (CaYSV), Cannaceae family.</t>
         </is>
       </c>
     </row>
@@ -2721,7 +2776,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Drought and salt stress affect the emission rates and composition of BVOC blends in urban trees, impacting plant interactions and the urban troposphere.</t>
+          <t>Drought and salt stress affect the emission rates and composition of biogenic volatile organic compounds (BVOCs) in urban trees, with specific changes in BVOC blends and herbivore-related bouquets.</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2731,7 +2786,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Quercus robur (Oak), Fagus sylvatica (Beech), Betula pendula (Birch), Carpinus betulus (Hornbeam)</t>
+          <t>Quercus robur (oak), Fagus sylvatica (beech), Betula pendula (silver birch), Carpinus betulus (hornbeam)</t>
         </is>
       </c>
     </row>
@@ -2751,7 +2806,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>A severe dieback of wild olive trees in Italy was found to be caused by Phytophthora species in the soil, including a newly reported species called P. bilorbang.</t>
+          <t>Severe dieback and mortality of wild olive trees in Italy caused by Phytophthora species, including the first report of P. bilorbang on wild olive trees.</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2762,10 +2817,10 @@
       <c r="F78" t="inlineStr">
         <is>
           <t>1. Wild olive trees (Olea europaea var. sylvestris)
-2. Ceratonia siliqua (used as bait for soil samples)
-3. Phytophthora species (unspecified)
-4. P. bilorbang (Phytophthora species)
-5. P. pseudocryptogea (Phytophthora species)</t>
+2. Ceratonia siliqua (used as bait)
+3. Phytophthora species
+4. P. bilorbang (CBS131653)
+5. P. pseudocryptogea (CBS139749)</t>
         </is>
       </c>
     </row>
@@ -2785,7 +2840,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>The study investigated the response of Juglans regia 'Sorrento' plants to saline irrigation, finding that the variety showed potential for cultivation in salinized soil due to its morpho-physiological resilience.</t>
+          <t>The study examined the effects of saltwater irrigation on Juglans regia 'Sorrento' plants. The plants showed no significant morphological or growth changes, indicating potential for cultivation in salinized environments.</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2815,7 +2870,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Increased fruit production in a fleshy-fruited tree promotes seedling recruitment both near and far, supporting both animal dispersal and predator satiation hypotheses. Population-level synchronization improves plant regeneration.</t>
+          <t>Masting increases fruit production in rowan trees, leading to higher seedling recruitment both near and far from rowans, supporting predator satiation and animal dispersal hypotheses.</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2826,8 +2881,9 @@
       <c r="F80" t="inlineStr">
         <is>
           <t>Species mentioned in the text:
-1. Rowan (Sorbus aucuparia, Rosaceae) - fleshy-fruited tree
-2. Heterospecific trees - other species of trees</t>
+1. Rowan (Sorbus aucuparia) - fleshy-fruited tree
+2. Heterospecifics - refers to non-conspecific trees in the vicinity
+3. Frugivores - animals that eat fruits and disperse seeds</t>
         </is>
       </c>
     </row>
@@ -2847,7 +2903,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>This article explores the use of soft cuttings to reproduce four species of the Elaeagnus genus, identifying effective growth regulators that improve root formation and shoot growth. These findings contribute to increasing biodiversity in Elaeagnus.</t>
+          <t>This article discusses the successful reproduction of four species of the Elaeagnus genus using soft cuttings and growth regulators, which could increase biodiversity in the genus.</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2857,7 +2913,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>species of the genus Elaeagnus L.</t>
+          <t>Four species of the genus Elaeagnus L.</t>
         </is>
       </c>
     </row>
@@ -2872,12 +2928,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>The Bryophytes of Europe Traits (BET) data set provides information on 65 traits and 25 bioclimatic variables related to bryophytes, offering a valuable resource for studying their biology, ecology, and conservation.</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2887,7 +2938,12 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Bryophytes</t>
+          <t>The species mentioned in the text are:
+1. Bryophytes (group of organisms)
+2. European Red List of bryophytes (specific list)
+3. Biological traits (related to life history, growth habit, sexual and vegetative reproduction)
+4. Ecological traits (indicator values, substrate, and habitat)
+5. Bioclimatic variables (based on the species' European range)</t>
         </is>
       </c>
     </row>
@@ -2907,7 +2963,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>A study on Tarenaya cultivars found low genetic diversity in seed-propagated cultivars and better flowering performance in vegetatively propagated ones. Further breeding is recommended to enhance variability.</t>
+          <t>A study on Tarenaya cultivars found low morphological diversity but clear genetic differentiation between seed-propagated and vegetatively propagated cultivars. Vegetatively propagated cultivars showed better performance.</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2917,10 +2973,9 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>1. Tarenaya hassleriana (syn. Cleome spinosa) - spider flower
-2. Tarenaya boliviensis
-3. Cleomaceae - family of spider flower
-4. tomato 'Stupicke' - internal standard for DNA content measurement</t>
+          <t>Species mentioned in the text:
+1. Tarenaya hassleriana (syn. Cleome spinosa)
+2. Tarenaya boliviensis</t>
         </is>
       </c>
     </row>
@@ -2940,7 +2995,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Compatibility of interspecific hybridization was tested between tulip cultivars and a wild species. Results showed varying success rates in terms of germination, receptivity, fruit-setting, seed germination and bulblet formation.</t>
+          <t>Interspecific hybridization between tulip cultivars and T. altaica showed varying compatibility in terms of germination, fruit-setting, and seed formation. T. altaica had the highest germination rate compared to other parents. Successful crosses included 'Heart of Poland' x T. altaica and 'Bolroyal Dream' x T. altaica.</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2950,12 +3005,12 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>- 'Heart of Poland' (Tulip cultivar)
-- 'Golden Parade' (Tulip cultivar)
-- 'Purple Dream' (Tulip cultivar)
-- 'Crystal Star' (Tulip cultivar)
-- 'Bolroyal Dream' (Tulip cultivar)
-- Tulipa altaica (Wild species)</t>
+          <t>1. Tulipa altaica 
+2. 'Heart of Poland' (tulip cultivar)
+3. 'Golden Parade' (tulip cultivar)
+4. 'Purple Dream' (tulip cultivar)
+5. 'Crystal Star' (tulip cultivar)
+6. 'Bolroyal Dream' (tulip cultivar)</t>
         </is>
       </c>
     </row>
@@ -3001,7 +3056,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Drought affects growth and quality of wild roses. Increasing deficit irrigation reduces plant growth, biomass yield, photosynthesis, and transpiration. Some wild roses are tolerant to drought.</t>
+          <t>A greenhouse experiment found that increasing drought stress reduced plant growth, yield, and quality in two Sicilian rose species. Identifying drought-tolerant roses could benefit nursery production in water-scarce regions.</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -3011,8 +3066,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>- Rosa canina L. (Wild rose)
-- Rosa sempervirens L. (Wild rose)</t>
+          <t>Rosa canina and Rosa sempervirens</t>
         </is>
       </c>
     </row>
@@ -3027,7 +3081,12 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>An ecological study in Istanbul evaluates how the physical properties of plant leaves affect sound absorption and attenuation in urban areas, using experimental data and statistical analysis.</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -3037,7 +3096,17 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>English Ivy (Hedera helix L.), Horse Chestnut (Aesculus hippocastanum L.), Hortensia (Hydrangea macrophylla (Thunb.) Ser.), Japanese Privet (Ligustrum japonicum Thunb.), Laurel (Laurus nobilis L.), Linden (Tilia tomentosa Moench), Magnolia (Magnolia grandiflora L.), Osmanthus (Osmanthus heterophyllus (G. Don) P.S. Green), Plane Tree (Platanus orientalis L.), and Cherry Laurel (Prunus laurocerasus L.)</t>
+          <t>Species mentioned in the text:
+1. English Ivy (Hedera helix L.)
+2. Horse Chestnut (Aesculus hippocastanum L.)
+3. Hortensia (Hydrangea macrophylla (Thunb.) Ser.)
+4. Japanese Privet (Ligustrum japonicum Thunb.)
+5. Laurel (Laurus nobilis L.)
+6. Linden (Tilia tomentosa Moench)
+7. Magnolia (Magnolia grandiflora L.)
+8. Osmanthus (Osmanthus heterophyllus (G. Don) P.S. Green)
+9. Plane Tree (Platanus orientalis L.)
+10. Cherry Laurel (Prunus laurocerasus L.)</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3126,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>This study explores hybridization between apple and pear, focusing on the effects of species and varietal differences on pollen tube growth, seed germination, and seedling survival. Prezygotic and postzygotic barriers are found in different crossing combinations. A marker for detecting intergeneric hybrids is also developed, aiding the development of hybrids with valuable traits.</t>
+          <t>The study explored the effects of species and varietal differences on pollination and hybrid seedling survival between apple and pear, highlighting prezygotic and postzygotic barriers, and providing potential markers for intergeneric hybrids.</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3067,9 +3136,11 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Species mentioned in the text:
-- Apple
-- Pear</t>
+          <t>- Apple (species)
+- Pear (species)
+- European pear (variety)
+- Japanese pear (variety)
+- Chinese pear (variety)</t>
         </is>
       </c>
     </row>
@@ -3089,7 +3160,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Filtered and unfiltered fish effluents were tested as organic fertilizers for onion yield and soil nutrients. Fish effluents performed better than horse manure, challenging the EU prohibition on their use in organic agriculture.</t>
+          <t>Fish effluents were tested as fertilisers for onion crops and found to enhance soil fertility and yield. The use of fish effluents may challenge current regulations on organic agriculture.</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -3099,15 +3170,14 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Species mentioned in the text:
-1. Onion (Allium cepa)
-2. Flavobacterium
-3. Pseudarthrobacter
-4. Sphingomonas
-5. Massilia
-6. Nitrososphaera
-7. Pseudomonas
-8. Nocardioides</t>
+          <t>- Onion (Allium cepa)
+- Flavobacterium
+- Pseudarthrobacter
+- Sphingomonas
+- Massilia
+- Nitrososphaera
+- Pseudomonas
+- Nocardioides</t>
         </is>
       </c>
     </row>
@@ -3127,7 +3197,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Growth and biomass production of young Norway spruce stands at lower altitudes in the Czech Republic were analyzed, highlighting the impact of climate change and recommending limited cultivation at specific altitudes and representation percentages.</t>
+          <t>The study examines the growth and biomass production of Norway spruce at lower altitudes in the Czech Republic, and recommends specific conditions for cultivation.</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3137,7 +3207,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>1. Norway spruce (Picea abies L. Karst)</t>
+          <t>Norway spruce (Picea abies L. Karst)</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3227,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Water limitation in the maternal environment during reproduction of Frangula alnus shrubs resulted in higher germination percentage and earlier seedling emergence, showing transgenerational effects. Population differentiation and genetic factors also influenced outcomes.</t>
+          <t>Water limitation during reproduction of Frangula alnus shrubs had transgenerational effects, increasing germination and advancing seedling emergence, with population differentiation in timing and germination stability.</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -3167,10 +3237,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>- Frangula alnus Mill. (shrub species)
-- Belgian provenance of Frangula alnus
-- Italian provenance of Frangula alnus
-- Swedish provenance of Frangula alnus</t>
+          <t>1. Frangula alnus</t>
         </is>
       </c>
     </row>
@@ -3190,7 +3257,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>A study in Portugal explored the use of phytotoxic waste extracts from invasive plants and agri-food waste as sustainable alternatives for urban weed control. The extracts showed potential in inhibiting weed germination and reducing post-emergence performance, but soil neutralized the effects. Combining these extracts with synthetic herbicides may be necessary for effective weed control.</t>
+          <t>Study in Portugal assessed the herbicidal potential of waste extracts from invasive plants (Acacia dealbata bark, Oxalis pes-caprae biomass) and agri-food (spent coffee grounds) on common urban weeds. Extracts reduced pre-emergence performance of weeds but had limited post-emergence effect. Soil neutralized pre-emergence effect, suggesting the need for additional synthetic herbicides in areas without soil. Combining bioherbicides and commercial formulations promotes sustainability.</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3215,7 +3282,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Bioslurry effluent was found to enhance the growth and quality of Swiss chard seedlings, with 100% and 200% application rates producing the best results.</t>
+          <t>Glasshouse experiments showed that fertilization with bioslurry at 100% and 200% rates improved the growth and quality of Swiss chard seedlings compared to inorganic fertilizers.</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3225,7 +3292,9 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Swiss chard (Beta vulgaris L.), Star 1801, Fordhook giant</t>
+          <t>- Swiss chard (Beta vulgaris L.)
+- Star 1801 (cultivar of Swiss chard)
+- Fordhook giant (cultivar of Swiss chard)</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3314,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Tomato brown rugose fruit virus (ToBRFV) poses a threat to global tomato production. Tests suggest that ToBRFV can be transmitted through contaminated seeds and water sources. Chemical and thermal sanitization methods have been found effective in controlling the virus.</t>
+          <t>Research in Mexico has identified Tomato brown rugose fruit virus (ToBRFV) in greenhouses and found that it can be transmitted through seed coats, seedlings, and water sources. Chemical and heat treatments were found to be effective in sanitizing growing media and utensils.</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3256,7 +3325,7 @@
       <c r="F94" t="inlineStr">
         <is>
           <t>1. Tomato brown rugose fruit virus (ToBRFV)
-2. Tomato</t>
+2. Nicotiana rustica</t>
         </is>
       </c>
     </row>
@@ -3276,7 +3345,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>The Canadian Plant Disease Survey highlights diseases in British Columbia in 2022, including nutrient deficiency, botrytis, and powdery mildew. No new diseases were found.</t>
+          <t>The Canadian Plant Disease Survey found that in 2022, cold, wet soils caused nutrient deficiency in plants, while cool, rainy weather led to high levels of botrytis in berries. Hot, dry weather in the following months caused heat and drought stress. Powdery mildew was also observed on many plants. No new diseases were found.</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3287,9 +3356,13 @@
       <c r="F95" t="inlineStr">
         <is>
           <t>Species mentioned in the text:
-1. Botrytis (causal agent)
-2. Powdery mildew (causal agent)
-3. Big-leaf maple (Acer macrophyllum)</t>
+1. Berry plants 
+2. Vegetable plants 
+3. Ornamental nursery plants 
+4. Landscape plants 
+5. Botrytis 
+6. Powdery mildew 
+7. Big-leaf maple (Acer macrophyllum)</t>
         </is>
       </c>
     </row>
@@ -3314,7 +3387,14 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Black turmeric (Curcuma Caesia Roxb.)</t>
+          <t>1. Black turmeric (Curcuma caesia)
+2. Staphylococcus aureus (bacterial strain)
+3. Escherichia coli (bacterial strain)
+4. Candida albicans (fungus strain)
+5. Human peroxiredoxin 5 (protein)
+6. Tyrosyl-tRNA synthetase from Staphylococcus aureus (protein)
+7. Glucosamine 6-phosphate synthase from Escherichia coli (protein)
+8. Zingiberaceae family</t>
         </is>
       </c>
     </row>
@@ -3334,7 +3414,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>The study evaluated the influence of living mulches on apple tree growth, yield, and fruit quality. Results showed that the cover crop affected tree growth and fruit characteristics, but tree tolerance improved with time. Specific factors like rootstocks and nursery stock quality played a significant role in apple tree tolerance to living mulches.</t>
+          <t>The study evaluated the long-term effects of living mulches on apple tree growth, yield, and fruit quality. It found that the presence of living mulch affected young tree growth and reduced fruit yield, but improved fruit coloration. The use of semidwarf rootstock, delayed sowing of the cover crop, and high-quality nursery stock were important for apple tree tolerance to living mulch.</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -3344,7 +3424,17 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>colonial bent grass (Agrostis vulgaris), white clover (Trifolium repens), blue fescue (Festuca ovina)</t>
+          <t>Species mentioned in the text:
+1. Colonial bent grass (Agrostis vulgaris)
+2. White clover (Trifolium repens)
+3. Blue fescue (Festuca ovina)
+4. Apple tree 'Ligol' (Malus)
+5. M.26 rootstock
+6. M.9 rootstock
+7. P 60 rootstock
+8. P 2 rootstock
+9. P 16 rootstock
+10. P 22 rootstock</t>
         </is>
       </c>
     </row>
@@ -3364,18 +3454,12 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Study investigates the effect of pear rootstocks and cultivars on leaf chlorophyll contents, growth, and yield. Canopy management with weaker growth improves chlorophyll content and yield performances.</t>
+          <t>Study investigates how different pear rootstocks and cultivars affect leaf chlorophyll content, growth, and yield. Results show significant differences and suggest canopy management can improve chlorophyll content and yield.</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>- European pear cultivars: 'Santa Maria', 'Williams', 'Deveci'
-- Rootstocks: BA29, QA, FOX9, FOX11, OHxF333, OHxF87, FAROLD40, Pyrus communis L. seedlings</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3395,7 +3479,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Different types of nitrogen fertilizer were tested on five varieties of lettuce to determine their effect on yield. Ammonium nitrate resulted in the highest lettuce weight and urea had the highest vitamin C content. Lettuce with red leaves had lower vitamin C content and higher nitrate accumulation.</t>
+          <t>The study investigated the impact of different nitrogen fertilizers on lettuce yield and quality. Ammonium nitrate resulted in the highest average weight and urea had the highest vitamin C content. Red lettuce varieties had lower vitamin C content and higher nitrate accumulation.</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3405,10 +3489,9 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>1. Lettuce (Lactuca sativa L.)
-2. Ammonium sulphate
-3. Ammonium nitrate
-4. Urea</t>
+          <t>Lettuce (Lactuca sativa L.)
+Varieties of lettuce: unidentified
+Nitrogen fertilizers: ammonium sulphate, ammonium nitrate, urea</t>
         </is>
       </c>
     </row>
@@ -3428,7 +3511,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>The use of nitrogen fertilization in apple trees can increase the risk of European canker, but its effect on fungal growth is unclear. Further research is needed for better fertilizer management.</t>
+          <t>Nitrogen fertilization in apple trees can boost plant growth but also increase the risk of European canker disease. Research is being conducted to determine the cause and find management strategies.</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3438,11 +3521,15 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>1. Apple (Malus domestica)
+          <t>1. Apple tree (Malus domestica)
 2. European canker (Neonectria ditissima)
 3. Fungal pathogen (Neonectria ditissima)
-4. Urea
-5. cv. Gala trees</t>
+4. Urea (a nitrogen-containing product)
+5. cv. Gala trees (a variety of apple tree)
+6. PDA (Potato Dextrose Agar, a growth medium)
+7. Leaf buds
+8. Spores
+9. Soil</t>
         </is>
       </c>
     </row>
@@ -3467,8 +3554,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>- European canker (Neonectria ditissima)
-- Apple trees (Malus domestica)</t>
+          <t>Neonectria ditissima</t>
         </is>
       </c>
     </row>

</xml_diff>